<commit_message>
Finish the basic of all forms except admin and delivery, need deep tests - docs uncomplete
</commit_message>
<xml_diff>
--- a/docs/SelfAssessment.xlsx
+++ b/docs/SelfAssessment.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MobileDistributionManagementSystem\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67B556C7-2839-4BF0-AD61-CC609DFDB600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,11 +24,106 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Use case diagrams</t>
+  </si>
+  <si>
+    <t>Use case specification</t>
+  </si>
+  <si>
+    <t>Rubrics</t>
+  </si>
+  <si>
+    <t>Completion</t>
+  </si>
+  <si>
+    <t>Contributor</t>
+  </si>
+  <si>
+    <t>1/ Project Management Plan</t>
+  </si>
+  <si>
+    <t>2/ Requirements Specification</t>
+  </si>
+  <si>
+    <t>3/ Architecture design</t>
+  </si>
+  <si>
+    <t>4/ Design</t>
+  </si>
+  <si>
+    <t>Mockup/Prototype</t>
+  </si>
+  <si>
+    <t>Class diagrams</t>
+  </si>
+  <si>
+    <t>Sequence diagrams</t>
+  </si>
+  <si>
+    <t>Database design</t>
+  </si>
+  <si>
+    <t>5/ Build apps with at least 4 main functions</t>
+  </si>
+  <si>
+    <t>6/ Coding Convention</t>
+  </si>
+  <si>
+    <t>7/ Testing, test case, Unit test</t>
+  </si>
+  <si>
+    <t>8/ SVN/GIT</t>
+  </si>
+  <si>
+    <t>9/ Report, demo</t>
+  </si>
+  <si>
+    <t>10/ High Distinction task</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>10 + 1</t>
+  </si>
+  <si>
+    <t>Nguyen Hoang Duy</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -49,13 +150,97 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -66,6 +251,19 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{887BBE6F-318D-4F89-8ED8-7368F9DEAD99}" name="Table1" displayName="Table1" ref="B4:E21" totalsRowShown="0" dataDxfId="2">
+  <autoFilter ref="B4:E21" xr:uid="{887BBE6F-318D-4F89-8ED8-7368F9DEAD99}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{45CD5DC1-869E-4340-B6CA-9EAFC74099B2}" name="Item" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{CBE3A4F5-80DF-4FB4-81BB-78EF2D07293D}" name="Rubrics" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{53498403-DA8E-49D1-A159-96E0A627E35A}" name="Completion" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{9E19E253-02A8-4372-AF3E-D208FD4708BB}" name="Contributor" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -330,13 +528,245 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B4:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="34.5703125" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="2">
+        <v>2</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="2">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="2">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Commit before update MSTest
</commit_message>
<xml_diff>
--- a/docs/SelfAssessment.xlsx
+++ b/docs/SelfAssessment.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MobileDistributionManagementSystem\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoang\OneDrive\Máy tính\MobileDistributionManagementSystem\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67B556C7-2839-4BF0-AD61-CC609DFDB600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F9006A3-C66A-4EC0-9568-3CF90F263450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -254,11 +254,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{887BBE6F-318D-4F89-8ED8-7368F9DEAD99}" name="Table1" displayName="Table1" ref="B4:E21" totalsRowShown="0" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{887BBE6F-318D-4F89-8ED8-7368F9DEAD99}" name="Table1" displayName="Table1" ref="B4:E21" totalsRowShown="0" dataDxfId="4">
   <autoFilter ref="B4:E21" xr:uid="{887BBE6F-318D-4F89-8ED8-7368F9DEAD99}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{45CD5DC1-869E-4340-B6CA-9EAFC74099B2}" name="Item" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{CBE3A4F5-80DF-4FB4-81BB-78EF2D07293D}" name="Rubrics" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{45CD5DC1-869E-4340-B6CA-9EAFC74099B2}" name="Item" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{CBE3A4F5-80DF-4FB4-81BB-78EF2D07293D}" name="Rubrics" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{53498403-DA8E-49D1-A159-96E0A627E35A}" name="Completion" dataDxfId="1"/>
     <tableColumn id="4" xr3:uid="{9E19E253-02A8-4372-AF3E-D208FD4708BB}" name="Contributor" dataDxfId="0"/>
   </tableColumns>
@@ -532,7 +532,7 @@
   <dimension ref="B4:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,7 +564,9 @@
       <c r="C5" s="2">
         <v>1</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="D5" s="2">
+        <v>0.75</v>
+      </c>
       <c r="E5" s="5" t="s">
         <v>22</v>
       </c>
@@ -588,7 +590,9 @@
       <c r="C7" s="1">
         <v>0.5</v>
       </c>
-      <c r="D7" s="1"/>
+      <c r="D7" s="1">
+        <v>0.25</v>
+      </c>
       <c r="E7" s="5" t="s">
         <v>22</v>
       </c>
@@ -600,7 +604,9 @@
       <c r="C8" s="1">
         <v>0.5</v>
       </c>
-      <c r="D8" s="1"/>
+      <c r="D8" s="1">
+        <v>0.25</v>
+      </c>
       <c r="E8" s="5" t="s">
         <v>22</v>
       </c>
@@ -612,7 +618,9 @@
       <c r="C9" s="2">
         <v>1</v>
       </c>
-      <c r="D9" s="1"/>
+      <c r="D9" s="2">
+        <v>0.5</v>
+      </c>
       <c r="E9" s="5" t="s">
         <v>22</v>
       </c>
@@ -636,7 +644,9 @@
       <c r="C11" s="1">
         <v>0.5</v>
       </c>
-      <c r="D11" s="1"/>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
       <c r="E11" s="5" t="s">
         <v>22</v>
       </c>
@@ -648,7 +658,9 @@
       <c r="C12" s="1">
         <v>0.5</v>
       </c>
-      <c r="D12" s="1"/>
+      <c r="D12" s="1">
+        <v>0.5</v>
+      </c>
       <c r="E12" s="5" t="s">
         <v>22</v>
       </c>
@@ -660,7 +672,9 @@
       <c r="C13" s="1">
         <v>0.5</v>
       </c>
-      <c r="D13" s="1"/>
+      <c r="D13" s="1">
+        <v>0.25</v>
+      </c>
       <c r="E13" s="5" t="s">
         <v>22</v>
       </c>
@@ -672,7 +686,9 @@
       <c r="C14" s="1">
         <v>0.5</v>
       </c>
-      <c r="D14" s="1"/>
+      <c r="D14" s="1">
+        <v>0.5</v>
+      </c>
       <c r="E14" s="5" t="s">
         <v>22</v>
       </c>
@@ -684,7 +700,9 @@
       <c r="C15" s="2">
         <v>2</v>
       </c>
-      <c r="D15" s="1"/>
+      <c r="D15" s="1">
+        <v>1.25</v>
+      </c>
       <c r="E15" s="5" t="s">
         <v>22</v>
       </c>
@@ -696,7 +714,9 @@
       <c r="C16" s="2">
         <v>0.5</v>
       </c>
-      <c r="D16" s="1"/>
+      <c r="D16" s="1">
+        <v>0.25</v>
+      </c>
       <c r="E16" s="5" t="s">
         <v>22</v>
       </c>
@@ -708,7 +728,9 @@
       <c r="C17" s="2">
         <v>1</v>
       </c>
-      <c r="D17" s="1"/>
+      <c r="D17" s="1">
+        <v>0.5</v>
+      </c>
       <c r="E17" s="5" t="s">
         <v>22</v>
       </c>
@@ -720,7 +742,9 @@
       <c r="C18" s="2">
         <v>0.5</v>
       </c>
-      <c r="D18" s="1"/>
+      <c r="D18" s="1">
+        <v>0.5</v>
+      </c>
       <c r="E18" s="5" t="s">
         <v>22</v>
       </c>
@@ -732,7 +756,9 @@
       <c r="C19" s="2">
         <v>1</v>
       </c>
-      <c r="D19" s="1"/>
+      <c r="D19" s="1">
+        <v>0.5</v>
+      </c>
       <c r="E19" s="5" t="s">
         <v>22</v>
       </c>
@@ -744,7 +770,9 @@
       <c r="C20" s="2">
         <v>1</v>
       </c>
-      <c r="D20" s="1"/>
+      <c r="D20" s="1">
+        <v>0</v>
+      </c>
       <c r="E20" s="5" t="s">
         <v>22</v>
       </c>
@@ -756,7 +784,9 @@
       <c r="C21" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="1"/>
+      <c r="D21" s="2">
+        <v>6</v>
+      </c>
       <c r="E21" s="5" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Final commit before submit
</commit_message>
<xml_diff>
--- a/docs/SelfAssessment.xlsx
+++ b/docs/SelfAssessment.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoang\OneDrive\Máy tính\MobileDistributionManagementSystem\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MobileDistributionManagementSystem\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F9006A3-C66A-4EC0-9568-3CF90F263450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F3358A9-FE42-42DE-AF26-3B9086ED3F12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -619,7 +619,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="2">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>22</v>
@@ -701,7 +701,7 @@
         <v>2</v>
       </c>
       <c r="D15" s="1">
-        <v>1.25</v>
+        <v>1</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>22</v>
@@ -757,7 +757,7 @@
         <v>1</v>
       </c>
       <c r="D19" s="1">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>22</v>
@@ -785,7 +785,7 @@
         <v>21</v>
       </c>
       <c r="D21" s="2">
-        <v>6</v>
+        <v>6.25</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>22</v>

</xml_diff>